<commit_message>
Add period validation feature
</commit_message>
<xml_diff>
--- a/Failed Invoices.xlsx
+++ b/Failed Invoices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LiBo3\PycharmProjects\PythonProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C9AE02-BE1E-49A1-BA86-2E809A9CA46E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0837044A-EF45-42F9-B50B-05EBBCB32E26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -347,7 +347,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B5"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed bug in Elexicon scanning
</commit_message>
<xml_diff>
--- a/Failed Invoices.xlsx
+++ b/Failed Invoices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LiBo3\PycharmProjects\PythonProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5099452D-CF22-437F-876D-4781C6B426A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F745CE5C-D96D-4A62-92D6-42D2CAA0AD8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -347,7 +347,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="A4" sqref="A2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added NTP and hydro one scanning methods
</commit_message>
<xml_diff>
--- a/Failed Invoices.xlsx
+++ b/Failed Invoices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LiBo3\PycharmProjects\PythonProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F745CE5C-D96D-4A62-92D6-42D2CAA0AD8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D16315-7A0B-484A-B93A-94C1BF0DD03B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -347,7 +347,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A2:B4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed bug in request for funding
</commit_message>
<xml_diff>
--- a/Failed Invoices.xlsx
+++ b/Failed Invoices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LiBo3\PycharmProjects\PythonProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D16315-7A0B-484A-B93A-94C1BF0DD03B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E70BDD-9E4C-40B6-9DCA-FB23612F44A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -347,7 +347,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added feature of naming invoice pdf by content and provided vendor name, in backend
</commit_message>
<xml_diff>
--- a/Failed Invoices.xlsx
+++ b/Failed Invoices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LiBo3\PycharmProjects\PythonProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E70BDD-9E4C-40B6-9DCA-FB23612F44A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7059D3-EE51-4048-84C6-419F7A68854F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -347,7 +347,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="A2:B2"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added vendor address change automation method
</commit_message>
<xml_diff>
--- a/Failed Invoices.xlsx
+++ b/Failed Invoices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LiBo3\PycharmProjects\PythonProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7059D3-EE51-4048-84C6-419F7A68854F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA104F62-D0CA-48A9-BB5C-BABB871CD24E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -347,7 +347,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="B3" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>